<commit_message>
Implemented Data driven testing for Add new class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -1,30 +1,220 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinza\LMS_Selenium\Team02_SeleniumNinjas\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB6F921-06C5-4954-B017-22D26E36ACBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-19310" yWindow="-760" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Home" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Program" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Batch" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Class" sheetId="5" r:id="rId8"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Home" sheetId="2" r:id="rId2"/>
+    <sheet name="Program" sheetId="3" r:id="rId3"/>
+    <sheet name="Batch" sheetId="4" r:id="rId4"/>
+    <sheet name="ClassDetailsForm" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
+  <si>
+    <t>NoofClasses</t>
+  </si>
+  <si>
+    <t>ClassTopic</t>
+  </si>
+  <si>
+    <t>ClassDescription</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Recording</t>
+  </si>
+  <si>
+    <t>AllMandateFieldsValidData</t>
+  </si>
+  <si>
+    <t>BatchName</t>
+  </si>
+  <si>
+    <t>StaffName</t>
+  </si>
+  <si>
+    <t>SelectClassDates</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Python101</t>
+  </si>
+  <si>
+    <t>arunasel S</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>02/21/2025,02/22/2025</t>
+  </si>
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>AllMandateFieldsInValidData</t>
+  </si>
+  <si>
+    <t>56yt</t>
+  </si>
+  <si>
+    <t>Y6</t>
+  </si>
+  <si>
+    <t>02/21/2025</t>
+  </si>
+  <si>
+    <t>sam</t>
+  </si>
+  <si>
+    <t>sqlserver12</t>
+  </si>
+  <si>
+    <t>ValidateNumOfClasses</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>BatchFieldReqVerification</t>
+  </si>
+  <si>
+    <t>ClassTopicReqVerification</t>
+  </si>
+  <si>
+    <t>ClassDatesReqVerification</t>
+  </si>
+  <si>
+    <t>StaffNameReqVerification</t>
+  </si>
+  <si>
+    <t>StatusReqVerification</t>
+  </si>
+  <si>
+    <t>appium</t>
+  </si>
+  <si>
+    <t>mobileTesting</t>
+  </si>
+  <si>
+    <t>programmingLanguage</t>
+  </si>
+  <si>
+    <t>javascript</t>
+  </si>
+  <si>
+    <t>locators</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>scripting</t>
+  </si>
+  <si>
+    <t>finding</t>
+  </si>
+  <si>
+    <t>forDynamic</t>
+  </si>
+  <si>
+    <t>deep knowledge</t>
+  </si>
+  <si>
+    <t>html path</t>
+  </si>
+  <si>
+    <t>frontend</t>
+  </si>
+  <si>
+    <t>easycoding</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>dataconnect</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>need</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -33,49 +223,90 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{781045EB-37F0-46FB-A02C-FC2F39F20785}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{948E5A86-F4AF-4777-8966-15A2DDCE16D1}"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -265,75 +496,352 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
-  <drawing r:id="rId1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented Edit Class and Delete class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinza\LMS_Selenium\Team02_SeleniumNinjas\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB6F921-06C5-4954-B017-22D26E36ACBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB264CE8-8B36-48AC-ADFE-C63DD02F0813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-760" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
   <si>
     <t>NoofClasses</t>
   </si>
@@ -62,33 +62,15 @@
     <t>Python101</t>
   </si>
   <si>
-    <t>arunasel S</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
-    <t>02/21/2025,02/22/2025</t>
-  </si>
-  <si>
     <t>TestCase</t>
   </si>
   <si>
-    <t>AllMandateFieldsInValidData</t>
-  </si>
-  <si>
-    <t>56yt</t>
-  </si>
-  <si>
     <t>Y6</t>
   </si>
   <si>
-    <t>02/21/2025</t>
-  </si>
-  <si>
-    <t>sam</t>
-  </si>
-  <si>
     <t>sqlserver12</t>
   </si>
   <si>
@@ -162,17 +144,48 @@
   </si>
   <si>
     <t>need</t>
+  </si>
+  <si>
+    <t>AllMandateFieldsValidDataForEdit</t>
+  </si>
+  <si>
+    <t>Java1212</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>ValidateInvalidMandatefields</t>
+  </si>
+  <si>
+    <t>03/20/2025,03/21/2025</t>
+  </si>
+  <si>
+    <t>Saranya M</t>
+  </si>
+  <si>
+    <t>Calculus3333</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -261,31 +274,31 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,22 +579,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -614,7 +628,7 @@
         <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -625,220 +639,250 @@
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
+      <c r="L2" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>44</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>44</v>
+      <c r="I4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="L4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>44</v>
+      <c r="I5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>25</v>
+      <c r="A6" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>44</v>
+      <c r="I6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>26</v>
+      <c r="A7" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="I7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>27</v>
+      <c r="A8" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="10" t="s">
+      <c r="J8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>44</v>
+      <c r="K8" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>28</v>
+      <c r="A9" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>37</v>
+      <c r="C9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>44</v>
+      <c r="L10" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commiting login,logout and dashboard functionality.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -1,30 +1,130 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\subha\git\Team02_SeleniumNinjasTech\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1FF00E-9BC4-48FF-AB18-E09127680950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Home" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Program" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Batch" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Class" sheetId="5" r:id="rId8"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Home" sheetId="2" r:id="rId2"/>
+    <sheet name="Program" sheetId="3" r:id="rId3"/>
+    <sheet name="Batch" sheetId="4" r:id="rId4"/>
+    <sheet name="Class" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Expected message</t>
+  </si>
+  <si>
+    <r>
+      <t>sdetnumpyninja</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2A00FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>@gmail.com</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Feb</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2A00FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>@2025</t>
+    </r>
+  </si>
+  <si>
+    <t>sdetnumpyninj@gmail.com</t>
+  </si>
+  <si>
+    <t>Feb@2024</t>
+  </si>
+  <si>
+    <t>Active User with given email Id Not Found</t>
+  </si>
+  <si>
+    <t>Bad credentials</t>
+  </si>
+  <si>
+    <t>Please enter your password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter your username </t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -33,49 +133,48 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -265,75 +364,143 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.453125" customWidth="1"/>
+    <col min="3" max="3" width="36.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B1E338CC-8806-4EAD-B746-4C6FAC84EA79}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{2770E1D2-75B1-43AE-A875-C660BBE7E357}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edit delete sort Program Module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\subha\git\Team02_SeleniumNinjasTech\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahaj\git\Team02_SeleniumNinjas\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1FF00E-9BC4-48FF-AB18-E09127680950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64711A3-666C-4301-A30A-E9607CBC614E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="2810" windowWidth="14400" windowHeight="7270" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Home" sheetId="2" r:id="rId2"/>
     <sheet name="Program" sheetId="3" r:id="rId3"/>
-    <sheet name="Batch" sheetId="4" r:id="rId4"/>
-    <sheet name="Class" sheetId="5" r:id="rId5"/>
+    <sheet name="AddProgram" sheetId="6" r:id="rId4"/>
+    <sheet name="Batch" sheetId="4" r:id="rId5"/>
+    <sheet name="Class" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -79,6 +80,36 @@
   </si>
   <si>
     <t xml:space="preserve">Please enter your username </t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>KarateSDET</t>
+  </si>
+  <si>
+    <t>ProgramName</t>
+  </si>
+  <si>
+    <t>ProgramDescription</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>FinalNinja</t>
   </si>
 </sst>
 </file>
@@ -150,9 +181,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -376,7 +407,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -465,17 +496,79 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187400F3-510A-4F63-8A96-9C22CAE56A9A}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -490,7 +583,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
Added some scenarios for class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinza\LMS_Selenium\Team02_SeleniumNinjas\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB264CE8-8B36-48AC-ADFE-C63DD02F0813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084F8E0C-42DA-4AED-A02E-38117122A9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-760" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Home" sheetId="2" r:id="rId2"/>
     <sheet name="Program" sheetId="3" r:id="rId3"/>
     <sheet name="Batch" sheetId="4" r:id="rId4"/>
-    <sheet name="ClassDetailsForm" sheetId="5" r:id="rId5"/>
+    <sheet name="Class" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>NoofClasses</t>
   </si>
@@ -167,18 +167,49 @@
     <t>Saranya M</t>
   </si>
   <si>
-    <t>Calculus3333</t>
+    <t>Saran</t>
+  </si>
+  <si>
+    <t>InvalidDataForMandatoryFieldsForEdit</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>SpecialCharValidationForEdit</t>
+  </si>
+  <si>
+    <t>%$*</t>
+  </si>
+  <si>
+    <t>#$*</t>
+  </si>
+  <si>
+    <t>#*^</t>
+  </si>
+  <si>
+    <t>AI_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -274,31 +305,33 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,15 +612,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
@@ -639,7 +672,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
@@ -648,7 +681,7 @@
       <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>46</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -674,7 +707,7 @@
       <c r="E3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>46</v>
       </c>
       <c r="H3" s="6" t="s">
@@ -697,7 +730,7 @@
       <c r="E4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>46</v>
       </c>
       <c r="H4" s="6" t="s">
@@ -729,7 +762,7 @@
       <c r="E5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -758,7 +791,7 @@
       <c r="E6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>46</v>
       </c>
       <c r="H6" s="6" t="s">
@@ -787,7 +820,7 @@
       <c r="D7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>46</v>
       </c>
       <c r="H7" s="6" t="s">
@@ -819,7 +852,7 @@
       <c r="E8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>46</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -851,7 +884,7 @@
       <c r="E9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>46</v>
       </c>
       <c r="I9" s="6" t="s">
@@ -866,7 +899,7 @@
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -875,7 +908,7 @@
       <c r="E10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>46</v>
       </c>
       <c r="H10" s="6" t="s">
@@ -883,6 +916,58 @@
       </c>
       <c r="L10" s="6" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11">
+        <v>234</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>